<commit_message>
[Angular][FilesMS] Update Import Product - Add Import WorkOrder
</commit_message>
<xml_diff>
--- a/Microservices/FilesMicroservice/Files.Api/wwwroot/test/ProductTemplate-test.xlsx
+++ b/Microservices/FilesMicroservice/Files.Api/wwwroot/test/ProductTemplate-test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khoa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khoa\Desktop\spatronics-shipping-application\Microservices\FilesMicroservice\Files.Api\wwwroot\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAA706E-34AE-49A4-9A40-C834B4900A34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2724184-D23C-458C-9D9D-EAB3745E99D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>ProductNumber</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>ABC2394984952</t>
+  </si>
+  <si>
+    <t>20000d</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D16:D17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -511,8 +514,8 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>20000</v>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -555,8 +558,8 @@
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
-        <v>20000</v>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -588,8 +591,8 @@
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1">
-        <v>20000</v>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -621,8 +624,8 @@
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="1">
-        <v>20000</v>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -665,8 +668,8 @@
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="1">
-        <v>20000</v>
+      <c r="C16" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -698,8 +701,8 @@
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="1">
-        <v>20000</v>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3">

</xml_diff>